<commit_message>
a catch up commit
</commit_message>
<xml_diff>
--- a/data/da_sampling/2014_crab_da_sampling_sites.xlsx
+++ b/data/da_sampling/2014_crab_da_sampling_sites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/dungeness/data/da_sampling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid/data/da_sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE46CCAB-24E3-9C40-A28B-AA601239B912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F6FC5F-67BD-0349-B832-8A74856375B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="4620" windowWidth="28040" windowHeight="17440" xr2:uid="{85CAFC41-C621-D94D-9406-458A45C0D7F8}"/>
+    <workbookView xWindow="31340" yWindow="1520" windowWidth="28040" windowHeight="17440" xr2:uid="{85CAFC41-C621-D94D-9406-458A45C0D7F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -212,7 +212,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -251,10 +251,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8BD7A6-83D4-0046-8F1A-9CA9FD54345E}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,303 +1136,303 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="4">
         <f>41+33/60</f>
         <v>41.55</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="4">
         <f>124+11/60</f>
         <v>124.18333333333334</v>
       </c>
-      <c r="G23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="G23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="4">
         <f>41+46/60</f>
         <v>41.766666666666666</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="4">
         <f>124+15/60</f>
         <v>124.25</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="4">
         <f>41+16/60</f>
         <v>41.266666666666666</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="4">
         <f>124+9/60</f>
         <v>124.15</v>
       </c>
-      <c r="G25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="G25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="D26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="4">
         <f>41+3/60</f>
         <v>41.05</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="4">
         <f>124+9/60</f>
         <v>124.15</v>
       </c>
-      <c r="G26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="G26" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="2">
+      <c r="D27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="4">
         <f>40+50/60</f>
         <v>40.833333333333336</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="4">
         <f>124+14/60</f>
         <v>124.23333333333333</v>
       </c>
-      <c r="G27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="G27" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="D28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="4">
         <f>40+39/60</f>
         <v>40.65</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="4">
         <f>124+23/60</f>
         <v>124.38333333333334</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="D29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="4">
         <f>39+48/60</f>
         <v>39.799999999999997</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="4">
         <f>123+53/60</f>
         <v>123.88333333333334</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="D30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="4">
         <f>39+52/60</f>
         <v>39.866666666666667</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="4">
         <f>123+57/60</f>
         <v>123.95</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="4">
         <f>38+26/60</f>
         <v>38.43333333333333</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="4">
         <f>123+11/60</f>
         <v>123.18333333333334</v>
       </c>
-      <c r="G31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="G31" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="4">
         <f>38+2/60</f>
         <v>38.033333333333331</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="4">
         <f>123+3/60</f>
         <v>123.05</v>
       </c>
-      <c r="G32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="G32" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="4">
         <f>37+50/60</f>
         <v>37.833333333333336</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="4">
         <f>122+46/60</f>
         <v>122.76666666666667</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="4">
         <f>37+37/60</f>
         <v>37.616666666666667</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="4">
         <f>122+41/60</f>
         <v>122.68333333333334</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="3" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>